<commit_message>
finished pcb rough draft and BoM
</commit_message>
<xml_diff>
--- a/Old_Clock/InfinityClock_BOM.xlsx
+++ b/Old_Clock/InfinityClock_BOM.xlsx
@@ -1,18 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huber\source\repos\infinity-mirror\Old_Clock\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC55B34-6B7A-4674-8C35-DAE911445C5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="17670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Complete BOM" sheetId="1" r:id="rId1"/>
     <sheet name="You buy" sheetId="2" r:id="rId2"/>
     <sheet name="You owe" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -278,7 +292,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#\ ???/???"/>
@@ -684,6 +698,27 @@
     <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -693,24 +728,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -725,9 +742,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -743,6 +757,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1034,26 +1051,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.69921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.796875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.296875" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.796875" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.19921875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="33"/>
       <c r="B1" s="31" t="s">
         <v>0</v>
@@ -1077,8 +1094,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="90" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="88" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="70" t="s">
@@ -1104,8 +1121,8 @@
         <v>0.9900000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="91"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="89"/>
       <c r="B3" s="74" t="s">
         <v>22</v>
       </c>
@@ -1129,8 +1146,8 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="92"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="90"/>
       <c r="B4" s="78" t="s">
         <v>51</v>
       </c>
@@ -1141,8 +1158,8 @@
       <c r="G4" s="80"/>
       <c r="H4" s="81"/>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="90" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="88" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="70" t="s">
@@ -1168,8 +1185,8 @@
         <v>8.3266666666666662</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="91"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="89"/>
       <c r="B6" s="74" t="s">
         <v>11</v>
       </c>
@@ -1193,8 +1210,8 @@
         <v>4.49</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="91"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="89"/>
       <c r="B7" s="74" t="s">
         <v>13</v>
       </c>
@@ -1218,8 +1235,8 @@
         <v>9.33</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="92"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="90"/>
       <c r="B8" s="78" t="s">
         <v>17</v>
       </c>
@@ -1238,8 +1255,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="93" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="91" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="70" t="s">
@@ -1265,8 +1282,8 @@
         <v>24.95</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="94"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="92"/>
       <c r="B10" s="74" t="s">
         <v>27</v>
       </c>
@@ -1289,8 +1306,8 @@
         <v>9.9499999999999993</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="94"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="92"/>
       <c r="B11" s="74" t="s">
         <v>60</v>
       </c>
@@ -1314,8 +1331,8 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="94"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="92"/>
       <c r="B12" s="74" t="s">
         <v>74</v>
       </c>
@@ -1339,8 +1356,8 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="94"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="92"/>
       <c r="B13" s="74" t="s">
         <v>50</v>
       </c>
@@ -1364,8 +1381,8 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="94"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="92"/>
       <c r="B14" s="5" t="s">
         <v>53</v>
       </c>
@@ -1392,8 +1409,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="94"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="92"/>
       <c r="B15" s="74" t="s">
         <v>29</v>
       </c>
@@ -1419,8 +1436,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="94"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="92"/>
       <c r="B16" s="74" t="s">
         <v>35</v>
       </c>
@@ -1444,8 +1461,8 @@
         <v>2.95</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="94"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="92"/>
       <c r="B17" s="74" t="s">
         <v>37</v>
       </c>
@@ -1469,8 +1486,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="94"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="92"/>
       <c r="B18" s="74" t="s">
         <v>39</v>
       </c>
@@ -1497,9 +1514,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="94"/>
-      <c r="B19" s="89" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="92"/>
+      <c r="B19" s="96" t="s">
         <v>31</v>
       </c>
       <c r="C19" s="75" t="s">
@@ -1522,9 +1539,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="94"/>
-      <c r="B20" s="89"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="92"/>
+      <c r="B20" s="96"/>
       <c r="C20" s="75" t="s">
         <v>66</v>
       </c>
@@ -1545,9 +1562,9 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="94"/>
-      <c r="B21" s="89"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="92"/>
+      <c r="B21" s="96"/>
       <c r="C21" s="75" t="s">
         <v>68</v>
       </c>
@@ -1568,9 +1585,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="94"/>
-      <c r="B22" s="89"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="92"/>
+      <c r="B22" s="96"/>
       <c r="C22" s="75" t="s">
         <v>67</v>
       </c>
@@ -1591,9 +1608,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="94"/>
-      <c r="B23" s="88" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="92"/>
+      <c r="B23" s="95" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="19" t="s">
@@ -1619,9 +1636,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="94"/>
-      <c r="B24" s="88"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="92"/>
+      <c r="B24" s="95"/>
       <c r="C24" s="75" t="s">
         <v>63</v>
       </c>
@@ -1645,9 +1662,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="94"/>
-      <c r="B25" s="88"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="92"/>
+      <c r="B25" s="95"/>
       <c r="C25" s="75" t="s">
         <v>64</v>
       </c>
@@ -1657,7 +1674,7 @@
       <c r="E25" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="101">
+      <c r="F25" s="87">
         <v>0.01</v>
       </c>
       <c r="G25" s="76">
@@ -1671,9 +1688,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="94"/>
-      <c r="B26" s="88"/>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="92"/>
+      <c r="B26" s="95"/>
       <c r="C26" s="4" t="s">
         <v>65</v>
       </c>
@@ -1697,8 +1714,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="94"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="92"/>
       <c r="B27" s="74" t="s">
         <v>41</v>
       </c>
@@ -1722,8 +1739,8 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="94"/>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="92"/>
       <c r="B28" s="74" t="s">
         <v>77</v>
       </c>
@@ -1747,8 +1764,8 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="94"/>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="92"/>
       <c r="B29" s="74" t="s">
         <v>76</v>
       </c>
@@ -1772,8 +1789,8 @@
         <v>2.8499999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="94"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="92"/>
       <c r="B30" s="5" t="s">
         <v>28</v>
       </c>
@@ -1797,9 +1814,9 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="94"/>
-      <c r="B31" s="89" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="92"/>
+      <c r="B31" s="96" t="s">
         <v>45</v>
       </c>
       <c r="C31" s="75" t="s">
@@ -1822,9 +1839,9 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="94"/>
-      <c r="B32" s="89"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="92"/>
+      <c r="B32" s="96"/>
       <c r="C32" s="75" t="s">
         <v>47</v>
       </c>
@@ -1845,9 +1862,9 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="94"/>
-      <c r="B33" s="89"/>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="92"/>
+      <c r="B33" s="96"/>
       <c r="C33" s="19" t="s">
         <v>52</v>
       </c>
@@ -1871,8 +1888,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="94"/>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="92"/>
       <c r="B34" s="74" t="s">
         <v>70</v>
       </c>
@@ -1896,8 +1913,8 @@
         <v>5.3166666666666664</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="95"/>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="93"/>
       <c r="B35" s="24" t="s">
         <v>72</v>
       </c>
@@ -1924,7 +1941,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B36" s="20"/>
       <c r="C36" s="19"/>
       <c r="D36" s="20"/>
@@ -1938,16 +1955,16 @@
         <v>124.76700000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C39">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
-      <c r="B40" s="87" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B40" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="87"/>
+      <c r="C40" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1970,26 +1987,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.296875" style="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.69921875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.296875" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.796875" style="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="25"/>
+    <col min="8" max="8" width="8.796875" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="33"/>
       <c r="B1" s="31" t="s">
         <v>0</v>
@@ -2013,8 +2030,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="93" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="91" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="20" t="s">
@@ -2040,8 +2057,8 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="94"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="92"/>
       <c r="B3" s="5" t="s">
         <v>28</v>
       </c>
@@ -2065,8 +2082,8 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="94"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="92"/>
       <c r="B4" s="20" t="s">
         <v>29</v>
       </c>
@@ -2089,8 +2106,8 @@
         <v>10.69</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="94"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="92"/>
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
@@ -2114,8 +2131,8 @@
         <v>24.95</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="94"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="92"/>
       <c r="B6" s="20" t="s">
         <v>27</v>
       </c>
@@ -2138,8 +2155,8 @@
         <v>9.9499999999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="94"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="92"/>
       <c r="B7" s="5" t="s">
         <v>74</v>
       </c>
@@ -2163,8 +2180,8 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="94"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="92"/>
       <c r="B8" s="20" t="s">
         <v>50</v>
       </c>
@@ -2188,8 +2205,8 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="94"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="92"/>
       <c r="B9" s="5" t="s">
         <v>53</v>
       </c>
@@ -2213,8 +2230,8 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="94"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="92"/>
       <c r="B10" s="20" t="s">
         <v>37</v>
       </c>
@@ -2238,8 +2255,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="94"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="92"/>
       <c r="B11" s="37" t="s">
         <v>31</v>
       </c>
@@ -2263,8 +2280,8 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="94"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="92"/>
       <c r="B12" s="20" t="s">
         <v>41</v>
       </c>
@@ -2288,8 +2305,8 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="94"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="92"/>
       <c r="B13" s="5" t="s">
         <v>77</v>
       </c>
@@ -2313,8 +2330,8 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="94"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="92"/>
       <c r="B14" s="20" t="s">
         <v>76</v>
       </c>
@@ -2338,9 +2355,9 @@
         <v>2.8499999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="94"/>
-      <c r="B15" s="96" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="92"/>
+      <c r="B15" s="97" t="s">
         <v>45</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -2363,9 +2380,9 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="94"/>
-      <c r="B16" s="96"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="92"/>
+      <c r="B16" s="97"/>
       <c r="C16" s="19" t="s">
         <v>47</v>
       </c>
@@ -2386,9 +2403,9 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="95"/>
-      <c r="B17" s="97"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="93"/>
+      <c r="B17" s="98"/>
       <c r="C17" s="12" t="s">
         <v>52</v>
       </c>
@@ -2409,7 +2426,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B18" s="20"/>
       <c r="C18" s="19"/>
       <c r="D18" s="20"/>
@@ -2438,26 +2455,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.296875" style="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="68" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="68" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" style="68" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.69921875" style="68" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.296875" style="68" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.796875" style="68" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" style="68" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="68"/>
+    <col min="8" max="8" width="8.796875" style="68"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="33"/>
       <c r="B1" s="31" t="s">
         <v>0</v>
@@ -2481,8 +2498,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="93" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="91" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -2508,8 +2525,8 @@
         <v>0.9900000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="94"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="92"/>
       <c r="B3" s="9" t="s">
         <v>22</v>
       </c>
@@ -2533,8 +2550,8 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="95"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="93"/>
       <c r="B4" s="13" t="s">
         <v>51</v>
       </c>
@@ -2545,8 +2562,8 @@
       <c r="G4" s="49"/>
       <c r="H4" s="50"/>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="98" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="99" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -2572,8 +2589,8 @@
         <v>8.3266666666666662</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="99"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="100"/>
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
@@ -2597,8 +2614,8 @@
         <v>4.49</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="99"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="100"/>
       <c r="B7" s="9" t="s">
         <v>13</v>
       </c>
@@ -2622,8 +2639,8 @@
         <v>9.33</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="100"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="101"/>
       <c r="B8" s="13" t="s">
         <v>17</v>
       </c>
@@ -2642,8 +2659,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="93" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="91" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -2669,9 +2686,9 @@
         <v>4.166666666666667</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="94"/>
-      <c r="B10" s="88" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="92"/>
+      <c r="B10" s="95" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -2694,9 +2711,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="94"/>
-      <c r="B11" s="88"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="92"/>
+      <c r="B11" s="95"/>
       <c r="C11" s="19" t="s">
         <v>68</v>
       </c>
@@ -2717,9 +2734,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="94"/>
-      <c r="B12" s="88"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="92"/>
+      <c r="B12" s="95"/>
       <c r="C12" s="4" t="s">
         <v>67</v>
       </c>
@@ -2740,9 +2757,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="94"/>
-      <c r="B13" s="89" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="92"/>
+      <c r="B13" s="96" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="19" t="s">
@@ -2765,9 +2782,9 @@
         <v>1.6633333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="94"/>
-      <c r="B14" s="89"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="92"/>
+      <c r="B14" s="96"/>
       <c r="C14" s="4" t="s">
         <v>63</v>
       </c>
@@ -2788,9 +2805,9 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="94"/>
-      <c r="B15" s="89"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="92"/>
+      <c r="B15" s="96"/>
       <c r="C15" s="19" t="s">
         <v>64</v>
       </c>
@@ -2811,9 +2828,9 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="94"/>
-      <c r="B16" s="89"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="92"/>
+      <c r="B16" s="96"/>
       <c r="C16" s="4" t="s">
         <v>65</v>
       </c>
@@ -2834,8 +2851,8 @@
         <v>0.18366666666666664</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="94"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="92"/>
       <c r="B17" s="20" t="s">
         <v>70</v>
       </c>
@@ -2859,8 +2876,8 @@
         <v>5.3166666666666664</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="95"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="93"/>
       <c r="B18" s="13" t="s">
         <v>72</v>
       </c>
@@ -2884,7 +2901,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B19" s="20"/>
       <c r="C19" s="19"/>
       <c r="D19" s="60"/>

</xml_diff>